<commit_message>
wire rates for the "short" benchmarks.
</commit_message>
<xml_diff>
--- a/papers/osdi14/ethernet-linerate.xlsx
+++ b/papers/osdi14/ethernet-linerate.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33140" yWindow="4780" windowWidth="27680" windowHeight="15720" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LINE RATE" sheetId="1" r:id="rId1"/>
     <sheet name="SHORT-TRANS" sheetId="2" r:id="rId2"/>
+    <sheet name="SHORT-TRANS (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="126">
   <si>
     <t>Gbps</t>
   </si>
@@ -335,6 +336,69 @@
   </si>
   <si>
     <t>Goodput [Gpbs]</t>
+  </si>
+  <si>
+    <t>Short benchmark -- IX</t>
+  </si>
+  <si>
+    <t>Note -- Linux has larger TCP headers (SOCK option, …)</t>
+  </si>
+  <si>
+    <t>54+size</t>
+  </si>
+  <si>
+    <t>RPC-REPLY</t>
+  </si>
+  <si>
+    <t>RPC-REQ</t>
+  </si>
+  <si>
+    <t>#roundtrips</t>
+  </si>
+  <si>
+    <t>#packets</t>
+  </si>
+  <si>
+    <t>n times</t>
+  </si>
+  <si>
+    <t>1 time</t>
+  </si>
+  <si>
+    <t># bytes</t>
+  </si>
+  <si>
+    <t>Packet wire time[ns]</t>
+  </si>
+  <si>
+    <t>total time [ns]</t>
+  </si>
+  <si>
+    <t>SHORT-SIZE benchmark</t>
+  </si>
+  <si>
+    <t>#rountrips=1</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>size/MTU</t>
+  </si>
+  <si>
+    <t>Packet wire time [ns]</t>
+  </si>
+  <si>
+    <t>Total time [ns]</t>
+  </si>
+  <si>
+    <t>M. TPS</t>
+  </si>
+  <si>
+    <t>SHORT-ROUNDTRIP BENCHMARKS Size=</t>
+  </si>
+  <si>
+    <t>Received is the bottlenecks; measuing goodput on Server RX.</t>
   </si>
 </sst>
 </file>
@@ -346,7 +410,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -388,6 +452,13 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -403,7 +474,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -411,8 +482,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="96">
+  <cellStyleXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -509,8 +660,52 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -521,8 +716,28 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="37" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="37" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="96">
+  <cellStyles count="140">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -570,6 +785,28 @@
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -617,6 +854,28 @@
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="37" builtinId="5"/>
   </cellStyles>
@@ -1709,10 +1968,996 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:L82"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" ht="18">
+      <c r="B3" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <v>74</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>74</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10">
+        <f>74+64</f>
+        <v>138</v>
+      </c>
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11">
+        <v>74</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12">
+        <f>74+64</f>
+        <v>138</v>
+      </c>
+      <c r="F12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13">
+        <v>74</v>
+      </c>
+      <c r="F13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14">
+        <v>74</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="4"/>
+      <c r="C23" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="4">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="12">
+        <v>64</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="15">
+        <v>1</v>
+      </c>
+      <c r="C29" s="15">
+        <v>2</v>
+      </c>
+      <c r="D29" s="15">
+        <v>4</v>
+      </c>
+      <c r="E29" s="15">
+        <v>8</v>
+      </c>
+      <c r="F29" s="15">
+        <v>16</v>
+      </c>
+      <c r="G29" s="15">
+        <v>32</v>
+      </c>
+      <c r="H29" s="15">
+        <v>64</v>
+      </c>
+      <c r="I29" s="15">
+        <v>128</v>
+      </c>
+      <c r="J29" s="16">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="18">
+        <f>4+(B29)</f>
+        <v>5</v>
+      </c>
+      <c r="C30" s="18">
+        <f t="shared" ref="C30:G30" si="0">4+(C29)</f>
+        <v>6</v>
+      </c>
+      <c r="D30" s="18">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E30" s="18">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F30" s="18">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="G30" s="18">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H30" s="18">
+        <f t="shared" ref="H30" si="1">4+(H29)</f>
+        <v>68</v>
+      </c>
+      <c r="I30" s="18">
+        <f t="shared" ref="I30" si="2">4+(I29)</f>
+        <v>132</v>
+      </c>
+      <c r="J30" s="19">
+        <f t="shared" ref="J30" si="3">4+(J29)</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="18">
+        <f>74+3*64+B29*118</f>
+        <v>384</v>
+      </c>
+      <c r="C31" s="18">
+        <f t="shared" ref="C31:G31" si="4">74+3*64+C29*118</f>
+        <v>502</v>
+      </c>
+      <c r="D31" s="18">
+        <f t="shared" si="4"/>
+        <v>738</v>
+      </c>
+      <c r="E31" s="18">
+        <f t="shared" si="4"/>
+        <v>1210</v>
+      </c>
+      <c r="F31" s="18">
+        <f t="shared" si="4"/>
+        <v>2154</v>
+      </c>
+      <c r="G31" s="18">
+        <f t="shared" si="4"/>
+        <v>4042</v>
+      </c>
+      <c r="H31" s="18">
+        <f t="shared" ref="H31:J31" si="5">74+3*64+H29*118</f>
+        <v>7818</v>
+      </c>
+      <c r="I31" s="18">
+        <f t="shared" si="5"/>
+        <v>15370</v>
+      </c>
+      <c r="J31" s="19">
+        <f t="shared" si="5"/>
+        <v>30474</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="18">
+        <f>B31*8/10</f>
+        <v>307.2</v>
+      </c>
+      <c r="C32" s="18">
+        <f t="shared" ref="C32:G32" si="6">C31*8/10</f>
+        <v>401.6</v>
+      </c>
+      <c r="D32" s="18">
+        <f t="shared" si="6"/>
+        <v>590.4</v>
+      </c>
+      <c r="E32" s="18">
+        <f t="shared" si="6"/>
+        <v>968</v>
+      </c>
+      <c r="F32" s="18">
+        <f t="shared" si="6"/>
+        <v>1723.2</v>
+      </c>
+      <c r="G32" s="18">
+        <f t="shared" si="6"/>
+        <v>3233.6</v>
+      </c>
+      <c r="H32" s="18">
+        <f t="shared" ref="H32" si="7">H31*8/10</f>
+        <v>6254.4</v>
+      </c>
+      <c r="I32" s="18">
+        <f t="shared" ref="I32" si="8">I31*8/10</f>
+        <v>12296</v>
+      </c>
+      <c r="J32" s="19">
+        <f t="shared" ref="J32" si="9">J31*8/10</f>
+        <v>24379.200000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
+      <c r="A33" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="18">
+        <f>B30*9.6</f>
+        <v>48</v>
+      </c>
+      <c r="C33" s="18">
+        <f t="shared" ref="C33:G33" si="10">C30*9.6</f>
+        <v>57.599999999999994</v>
+      </c>
+      <c r="D33" s="18">
+        <f t="shared" si="10"/>
+        <v>76.8</v>
+      </c>
+      <c r="E33" s="18">
+        <f t="shared" si="10"/>
+        <v>115.19999999999999</v>
+      </c>
+      <c r="F33" s="18">
+        <f t="shared" si="10"/>
+        <v>192</v>
+      </c>
+      <c r="G33" s="18">
+        <f t="shared" si="10"/>
+        <v>345.59999999999997</v>
+      </c>
+      <c r="H33" s="18">
+        <f t="shared" ref="H33:J33" si="11">H30*9.6</f>
+        <v>652.79999999999995</v>
+      </c>
+      <c r="I33" s="18">
+        <f t="shared" si="11"/>
+        <v>1267.2</v>
+      </c>
+      <c r="J33" s="19">
+        <f t="shared" si="11"/>
+        <v>2496</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
+      <c r="A34" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B34" s="18">
+        <f>B32+B33</f>
+        <v>355.2</v>
+      </c>
+      <c r="C34" s="18">
+        <f t="shared" ref="C34:G34" si="12">C32+C33</f>
+        <v>459.20000000000005</v>
+      </c>
+      <c r="D34" s="18">
+        <f t="shared" si="12"/>
+        <v>667.19999999999993</v>
+      </c>
+      <c r="E34" s="18">
+        <f t="shared" si="12"/>
+        <v>1083.2</v>
+      </c>
+      <c r="F34" s="18">
+        <f t="shared" si="12"/>
+        <v>1915.2</v>
+      </c>
+      <c r="G34" s="18">
+        <f t="shared" si="12"/>
+        <v>3579.2</v>
+      </c>
+      <c r="H34" s="18">
+        <f t="shared" ref="H34" si="13">H32+H33</f>
+        <v>6907.2</v>
+      </c>
+      <c r="I34" s="18">
+        <f t="shared" ref="I34" si="14">I32+I33</f>
+        <v>13563.2</v>
+      </c>
+      <c r="J34" s="19">
+        <f t="shared" ref="J34" si="15">J32+J33</f>
+        <v>26875.200000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" s="26">
+        <f>1000*B29/B34</f>
+        <v>2.8153153153153152</v>
+      </c>
+      <c r="C35" s="26">
+        <f t="shared" ref="C35:G35" si="16">1000*C29/C34</f>
+        <v>4.3554006968641108</v>
+      </c>
+      <c r="D35" s="26">
+        <f t="shared" si="16"/>
+        <v>5.9952038369304566</v>
+      </c>
+      <c r="E35" s="26">
+        <f t="shared" si="16"/>
+        <v>7.385524372230428</v>
+      </c>
+      <c r="F35" s="26">
+        <f t="shared" si="16"/>
+        <v>8.3542188805346704</v>
+      </c>
+      <c r="G35" s="26">
+        <f t="shared" si="16"/>
+        <v>8.9405453732677707</v>
+      </c>
+      <c r="H35" s="26">
+        <f t="shared" ref="H35" si="17">1000*H29/H34</f>
+        <v>9.26569376882094</v>
+      </c>
+      <c r="I35" s="26">
+        <f t="shared" ref="I35" si="18">1000*I29/I34</f>
+        <v>9.437300931933466</v>
+      </c>
+      <c r="J35" s="28">
+        <f t="shared" ref="J35" si="19">1000*J29/J34</f>
+        <v>9.5255105078287787</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
+      <c r="A36" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="B36" s="23">
+        <f>B35*64*8/1000</f>
+        <v>1.4414414414414414</v>
+      </c>
+      <c r="C36" s="23">
+        <f t="shared" ref="C36:J36" si="20">C35*64*8/1000</f>
+        <v>2.2299651567944245</v>
+      </c>
+      <c r="D36" s="23">
+        <f t="shared" si="20"/>
+        <v>3.0695443645083937</v>
+      </c>
+      <c r="E36" s="23">
+        <f t="shared" si="20"/>
+        <v>3.7813884785819791</v>
+      </c>
+      <c r="F36" s="23">
+        <f t="shared" si="20"/>
+        <v>4.2773600668337517</v>
+      </c>
+      <c r="G36" s="23">
+        <f t="shared" si="20"/>
+        <v>4.5775592311130984</v>
+      </c>
+      <c r="H36" s="23">
+        <f t="shared" si="20"/>
+        <v>4.744035209636321</v>
+      </c>
+      <c r="I36" s="23">
+        <f t="shared" si="20"/>
+        <v>4.8318980771499342</v>
+      </c>
+      <c r="J36" s="24">
+        <f t="shared" si="20"/>
+        <v>4.8770613800083344</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
+      <c r="A38" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="13"/>
+    </row>
+    <row r="39" spans="1:10">
+      <c r="A39" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B39" s="15">
+        <v>64</v>
+      </c>
+      <c r="C39" s="15">
+        <v>128</v>
+      </c>
+      <c r="D39" s="15">
+        <f>C39*2</f>
+        <v>256</v>
+      </c>
+      <c r="E39" s="15">
+        <f t="shared" ref="E39:J39" si="21">D39*2</f>
+        <v>512</v>
+      </c>
+      <c r="F39" s="15">
+        <f t="shared" si="21"/>
+        <v>1024</v>
+      </c>
+      <c r="G39" s="15">
+        <f t="shared" si="21"/>
+        <v>2048</v>
+      </c>
+      <c r="H39" s="15">
+        <f t="shared" si="21"/>
+        <v>4096</v>
+      </c>
+      <c r="I39" s="15">
+        <f t="shared" si="21"/>
+        <v>8192</v>
+      </c>
+      <c r="J39" s="16">
+        <f t="shared" si="21"/>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
+      <c r="A40" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40" s="18">
+        <f>B39/1460</f>
+        <v>4.3835616438356165E-2</v>
+      </c>
+      <c r="C40" s="18">
+        <f t="shared" ref="C40:J40" si="22">C39/1460</f>
+        <v>8.7671232876712329E-2</v>
+      </c>
+      <c r="D40" s="18">
+        <f t="shared" si="22"/>
+        <v>0.17534246575342466</v>
+      </c>
+      <c r="E40" s="18">
+        <f t="shared" si="22"/>
+        <v>0.35068493150684932</v>
+      </c>
+      <c r="F40" s="18">
+        <f t="shared" si="22"/>
+        <v>0.70136986301369864</v>
+      </c>
+      <c r="G40" s="18">
+        <f t="shared" si="22"/>
+        <v>1.4027397260273973</v>
+      </c>
+      <c r="H40" s="18">
+        <f t="shared" si="22"/>
+        <v>2.8054794520547945</v>
+      </c>
+      <c r="I40" s="18">
+        <f t="shared" si="22"/>
+        <v>5.6109589041095891</v>
+      </c>
+      <c r="J40" s="19">
+        <f t="shared" si="22"/>
+        <v>11.221917808219178</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="18">
+        <f>4+ROUNDUP(B40,0)</f>
+        <v>5</v>
+      </c>
+      <c r="C41" s="18">
+        <f t="shared" ref="C41:J41" si="23">4+ROUNDUP(C40,0)</f>
+        <v>5</v>
+      </c>
+      <c r="D41" s="18">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="E41" s="18">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="F41" s="18">
+        <f t="shared" si="23"/>
+        <v>5</v>
+      </c>
+      <c r="G41" s="18">
+        <f t="shared" si="23"/>
+        <v>6</v>
+      </c>
+      <c r="H41" s="18">
+        <f t="shared" si="23"/>
+        <v>7</v>
+      </c>
+      <c r="I41" s="18">
+        <f t="shared" si="23"/>
+        <v>10</v>
+      </c>
+      <c r="J41" s="19">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
+      <c r="A42" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B42" s="18">
+        <f>384-64+56*(B41-5)+B39</f>
+        <v>384</v>
+      </c>
+      <c r="C42" s="18">
+        <f t="shared" ref="C42:J42" si="24">384-64+56*(C41-5)+C39</f>
+        <v>448</v>
+      </c>
+      <c r="D42" s="18">
+        <f t="shared" si="24"/>
+        <v>576</v>
+      </c>
+      <c r="E42" s="18">
+        <f t="shared" si="24"/>
+        <v>832</v>
+      </c>
+      <c r="F42" s="18">
+        <f t="shared" si="24"/>
+        <v>1344</v>
+      </c>
+      <c r="G42" s="18">
+        <f t="shared" si="24"/>
+        <v>2424</v>
+      </c>
+      <c r="H42" s="18">
+        <f t="shared" si="24"/>
+        <v>4528</v>
+      </c>
+      <c r="I42" s="18">
+        <f t="shared" si="24"/>
+        <v>8792</v>
+      </c>
+      <c r="J42" s="19">
+        <f t="shared" si="24"/>
+        <v>17320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="18">
+        <f>B42*8/10</f>
+        <v>307.2</v>
+      </c>
+      <c r="C43" s="18">
+        <f t="shared" ref="C43:J43" si="25">C42*8/10</f>
+        <v>358.4</v>
+      </c>
+      <c r="D43" s="18">
+        <f t="shared" si="25"/>
+        <v>460.8</v>
+      </c>
+      <c r="E43" s="18">
+        <f t="shared" si="25"/>
+        <v>665.6</v>
+      </c>
+      <c r="F43" s="18">
+        <f t="shared" si="25"/>
+        <v>1075.2</v>
+      </c>
+      <c r="G43" s="18">
+        <f t="shared" si="25"/>
+        <v>1939.2</v>
+      </c>
+      <c r="H43" s="18">
+        <f t="shared" si="25"/>
+        <v>3622.4</v>
+      </c>
+      <c r="I43" s="18">
+        <f t="shared" si="25"/>
+        <v>7033.6</v>
+      </c>
+      <c r="J43" s="19">
+        <f t="shared" si="25"/>
+        <v>13856</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="18">
+        <f>B41*9.6</f>
+        <v>48</v>
+      </c>
+      <c r="C44" s="18">
+        <f t="shared" ref="C44:J44" si="26">C41*9.6</f>
+        <v>48</v>
+      </c>
+      <c r="D44" s="18">
+        <f t="shared" si="26"/>
+        <v>48</v>
+      </c>
+      <c r="E44" s="18">
+        <f t="shared" si="26"/>
+        <v>48</v>
+      </c>
+      <c r="F44" s="18">
+        <f t="shared" si="26"/>
+        <v>48</v>
+      </c>
+      <c r="G44" s="18">
+        <f t="shared" si="26"/>
+        <v>57.599999999999994</v>
+      </c>
+      <c r="H44" s="18">
+        <f t="shared" si="26"/>
+        <v>67.2</v>
+      </c>
+      <c r="I44" s="18">
+        <f t="shared" si="26"/>
+        <v>96</v>
+      </c>
+      <c r="J44" s="19">
+        <f t="shared" si="26"/>
+        <v>153.6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="18">
+        <f>B43+B44</f>
+        <v>355.2</v>
+      </c>
+      <c r="C45" s="18">
+        <f t="shared" ref="C45:J45" si="27">C43+C44</f>
+        <v>406.4</v>
+      </c>
+      <c r="D45" s="18">
+        <f t="shared" si="27"/>
+        <v>508.8</v>
+      </c>
+      <c r="E45" s="18">
+        <f t="shared" si="27"/>
+        <v>713.6</v>
+      </c>
+      <c r="F45" s="18">
+        <f t="shared" si="27"/>
+        <v>1123.2</v>
+      </c>
+      <c r="G45" s="18">
+        <f t="shared" si="27"/>
+        <v>1996.8</v>
+      </c>
+      <c r="H45" s="18">
+        <f t="shared" si="27"/>
+        <v>3689.6</v>
+      </c>
+      <c r="I45" s="18">
+        <f t="shared" si="27"/>
+        <v>7129.6</v>
+      </c>
+      <c r="J45" s="19">
+        <f t="shared" si="27"/>
+        <v>14009.6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="26">
+        <f>1000/B45</f>
+        <v>2.8153153153153152</v>
+      </c>
+      <c r="C46" s="26">
+        <f t="shared" ref="C46:J46" si="28">1000/C45</f>
+        <v>2.4606299212598426</v>
+      </c>
+      <c r="D46" s="26">
+        <f t="shared" si="28"/>
+        <v>1.9654088050314464</v>
+      </c>
+      <c r="E46" s="26">
+        <f t="shared" si="28"/>
+        <v>1.4013452914798206</v>
+      </c>
+      <c r="F46" s="26">
+        <f t="shared" si="28"/>
+        <v>0.8903133903133903</v>
+      </c>
+      <c r="G46" s="26">
+        <f t="shared" si="28"/>
+        <v>0.50080128205128205</v>
+      </c>
+      <c r="H46" s="26">
+        <f t="shared" si="28"/>
+        <v>0.2710320901994796</v>
+      </c>
+      <c r="I46" s="26">
+        <f t="shared" si="28"/>
+        <v>0.14026032315978457</v>
+      </c>
+      <c r="J46" s="28">
+        <f t="shared" si="28"/>
+        <v>7.1379625399725907E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="23">
+        <f>B46*B39*8/1000</f>
+        <v>1.4414414414414414</v>
+      </c>
+      <c r="C47" s="23">
+        <f t="shared" ref="C47:J47" si="29">C46*C39*8/1000</f>
+        <v>2.5196850393700787</v>
+      </c>
+      <c r="D47" s="23">
+        <f t="shared" si="29"/>
+        <v>4.0251572327044025</v>
+      </c>
+      <c r="E47" s="23">
+        <f t="shared" si="29"/>
+        <v>5.739910313901345</v>
+      </c>
+      <c r="F47" s="23">
+        <f t="shared" si="29"/>
+        <v>7.2934472934472936</v>
+      </c>
+      <c r="G47" s="23">
+        <f t="shared" si="29"/>
+        <v>8.2051282051282044</v>
+      </c>
+      <c r="H47" s="23">
+        <f t="shared" si="29"/>
+        <v>8.8811795316565476</v>
+      </c>
+      <c r="I47" s="23">
+        <f t="shared" si="29"/>
+        <v>9.1921005385996413</v>
+      </c>
+      <c r="J47" s="24">
+        <f t="shared" si="29"/>
+        <v>9.3558702603928747</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="B48" s="6"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:12">
+      <c r="B50" s="7"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="K50" s="8"/>
+    </row>
+    <row r="53" spans="1:12">
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="B66" s="6"/>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="B78" s="6"/>
+    </row>
+    <row r="82" spans="3:4">
+      <c r="C82" s="7"/>
+      <c r="D82" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>